<commit_message>
Reorganized docs folder. Updated framework doc.
</commit_message>
<xml_diff>
--- a/docs/fsm-trace.xlsx
+++ b/docs/fsm-trace.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\hovercam\ultra12\software\microblaze\firmware\ultra12\docs\state-machine-framework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\fsm\state-machine-framework\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="39">
   <si>
     <t>consumed</t>
   </si>
@@ -30,21 +30,12 @@
     <t>EVT_FSM_ENTRY</t>
   </si>
   <si>
-    <t>ignored</t>
-  </si>
-  <si>
     <t>not_consumed</t>
   </si>
   <si>
-    <t>enter</t>
-  </si>
-  <si>
     <t>top</t>
   </si>
   <si>
-    <t>exit</t>
-  </si>
-  <si>
     <t>run</t>
   </si>
   <si>
@@ -66,67 +57,85 @@
     <t>Status</t>
   </si>
   <si>
-    <t>MyFsmInit</t>
-  </si>
-  <si>
     <t>init</t>
   </si>
   <si>
-    <t>MyFsmStateHandleEvent</t>
-  </si>
-  <si>
-    <t>TopState1</t>
-  </si>
-  <si>
-    <t>EVT_1</t>
-  </si>
-  <si>
-    <t>TopState2</t>
-  </si>
-  <si>
-    <t>EVT_2</t>
-  </si>
-  <si>
-    <t>EVT_3</t>
-  </si>
-  <si>
-    <t>EVT_4</t>
-  </si>
-  <si>
-    <t>MyFsmRun</t>
-  </si>
-  <si>
-    <t>nested_1</t>
-  </si>
-  <si>
-    <t>Nested1State1</t>
-  </si>
-  <si>
-    <t>MyNestedFsm1State1Evt_Entry</t>
-  </si>
-  <si>
-    <t>entry_actions</t>
-  </si>
-  <si>
     <t>EVT_FSM_SUPERSTATE_ENTRY</t>
   </si>
   <si>
-    <t>EVT_FSM_SUPERSTATE_EXIT</t>
-  </si>
-  <si>
-    <t>nested_2</t>
-  </si>
-  <si>
-    <t>Nested2State1</t>
-  </si>
-  <si>
-    <t>MyNestedFsm2State1Evt_Entry</t>
-  </si>
-  <si>
-    <t>Nested2State2</t>
-  </si>
-  <si>
-    <t>Nested1State2</t>
+    <t>SdhcFsmInit</t>
+  </si>
+  <si>
+    <t>CoordFsmInit</t>
+  </si>
+  <si>
+    <t>CoordFsmStateHandleEvent</t>
+  </si>
+  <si>
+    <t>begin</t>
+  </si>
+  <si>
+    <t>Idle</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>SdhcFsmStateHandleEvent</t>
+  </si>
+  <si>
+    <t>Ready</t>
+  </si>
+  <si>
+    <t>playback</t>
+  </si>
+  <si>
+    <t>FileClosed</t>
+  </si>
+  <si>
+    <t>capture</t>
+  </si>
+  <si>
+    <t>FileOpen</t>
+  </si>
+  <si>
+    <t>NotReady</t>
+  </si>
+  <si>
+    <t>EVT_DMA_JPEG_FRAME_COMPLETE</t>
+  </si>
+  <si>
+    <t>DmaShutdown</t>
+  </si>
+  <si>
+    <t>EVT_SDHC_FILE_CLOSE</t>
+  </si>
+  <si>
+    <t>EVT_COORD_DMA_DONE</t>
+  </si>
+  <si>
+    <t>EVT_COORD_LIVE_PLAY_BEGIN</t>
+  </si>
+  <si>
+    <t>LivePlay</t>
+  </si>
+  <si>
+    <t>liveplay</t>
+  </si>
+  <si>
+    <t>EVT_COORD_STILL_IMAGE_CAPTURE</t>
+  </si>
+  <si>
+    <t>StillCapture</t>
+  </si>
+  <si>
+    <t>EVT_SDHC_CAPTURE_FILE_OPEN</t>
+  </si>
+  <si>
+    <t>CaptureDone</t>
+  </si>
+  <si>
+    <t>EVT_COORD_CAPTURE_DONE</t>
   </si>
 </sst>
 </file>
@@ -667,7 +676,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -693,53 +702,6 @@
     <dxf>
       <font>
         <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
       </font>
     </dxf>
     <dxf>
@@ -1038,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,22 +1018,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1079,21 +1041,21 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
@@ -1104,112 +1066,118 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
       </c>
-      <c r="F7" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>
@@ -1220,360 +1188,369 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="E16" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="E17" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="F17" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
         <v>18</v>
       </c>
       <c r="E18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D19" t="s">
         <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
         <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E23" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E24" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F25" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="D26" t="s">
         <v>18</v>
       </c>
       <c r="E26" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="F26" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="D27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D28" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E28" t="s">
-        <v>29</v>
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="s">
         <v>33</v>
       </c>
-      <c r="B29" t="s">
-        <v>8</v>
+      <c r="D29" t="s">
+        <v>35</v>
       </c>
       <c r="E29" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D30" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E30" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="F30" t="s">
         <v>0</v>
@@ -1581,19 +1558,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E31" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="F31" t="s">
         <v>0</v>
@@ -1601,53 +1578,53 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E32" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D33" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E33" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C34" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D34" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E34" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="F34" t="s">
         <v>0</v>
@@ -1655,16 +1632,16 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C35" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D35" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E35" t="s">
         <v>1</v>
@@ -1672,36 +1649,36 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C36" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D36" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E36" t="s">
         <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B37" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C37" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D37" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E37" t="s">
         <v>2</v>
@@ -1709,315 +1686,315 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C38" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D38" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E38" t="s">
         <v>2</v>
       </c>
       <c r="F38" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D39" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E39" t="s">
-        <v>22</v>
-      </c>
-      <c r="F39" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D40" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E40" t="s">
-        <v>21</v>
+        <v>36</v>
+      </c>
+      <c r="F40" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C41" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D41" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E41" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C42" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D42" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E42" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="F42" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D43" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E43" t="s">
-        <v>21</v>
-      </c>
-      <c r="F43" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C44" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D44" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E44" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F44" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C45" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E45" t="s">
-        <v>30</v>
+        <v>36</v>
+      </c>
+      <c r="F45" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C46" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E46" t="s">
-        <v>30</v>
-      </c>
-      <c r="F46" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D47" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E47" t="s">
-        <v>1</v>
-      </c>
-      <c r="F47" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D48" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E48" t="s">
-        <v>2</v>
+        <v>27</v>
+      </c>
+      <c r="F48" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C49" t="s">
+        <v>24</v>
+      </c>
+      <c r="D49" t="s">
         <v>25</v>
       </c>
-      <c r="D49" t="s">
-        <v>35</v>
-      </c>
       <c r="E49" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C50" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50" t="s">
         <v>25</v>
       </c>
-      <c r="D50" t="s">
-        <v>35</v>
-      </c>
       <c r="E50" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F50" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C51" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D51" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E51" t="s">
-        <v>2</v>
-      </c>
-      <c r="F51" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C52" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D52" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E52" t="s">
-        <v>23</v>
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D53" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E53" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C54" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D54" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E54" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="F54" t="s">
         <v>0</v>
@@ -2025,269 +2002,275 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C55" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D55" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="E55" t="s">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="F55" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C56" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D56" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E56" t="s">
-        <v>1</v>
-      </c>
-      <c r="F56" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B57" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C57" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D57" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E57" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B58" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+      <c r="C58" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" t="s">
+        <v>35</v>
       </c>
       <c r="E58" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="F58" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B59" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C59" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D59" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E59" t="s">
-        <v>2</v>
-      </c>
-      <c r="F59" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C60" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="D60" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="E60" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="F60" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B61" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C61" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="D61" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E61" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C62" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D62" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E62" t="s">
-        <v>19</v>
+        <v>2</v>
+      </c>
+      <c r="F62" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C63" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D63" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E63" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="F63" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B64" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C64" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D64" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E64" t="s">
-        <v>19</v>
-      </c>
-      <c r="F64" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B65" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C65" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D65" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E65" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B66" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C66" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D66" t="s">
         <v>26</v>
       </c>
       <c r="E66" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="F66" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B67" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C67" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D67" t="s">
         <v>26</v>
       </c>
       <c r="E67" t="s">
-        <v>30</v>
-      </c>
-      <c r="F67" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B68" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C68" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D68" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E68" t="s">
         <v>1</v>
       </c>
       <c r="F68" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B69" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C69" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E69" t="s">
         <v>2</v>
@@ -2295,44 +2278,53 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C70" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D70" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E70" t="s">
-        <v>29</v>
+        <v>2</v>
+      </c>
+      <c r="F70" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B71" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="C71" t="s">
+        <v>24</v>
+      </c>
+      <c r="D71" t="s">
+        <v>37</v>
       </c>
       <c r="E71" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B72" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C72" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D72" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E72" t="s">
         <v>29</v>
@@ -2343,148 +2335,276 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B73" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C73" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D73" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="E73" t="s">
-        <v>2</v>
-      </c>
-      <c r="F73" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C74" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D74" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="E74" t="s">
-        <v>23</v>
+        <v>1</v>
+      </c>
+      <c r="F74" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B75" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C75" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D75" t="s">
         <v>32</v>
       </c>
       <c r="E75" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B76" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C76" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D76" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E76" t="s">
-        <v>23</v>
-      </c>
-      <c r="F76" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B77" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C77" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D77" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E77" t="s">
-        <v>23</v>
-      </c>
-      <c r="F77" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>20</v>
+      </c>
+      <c r="B78" t="s">
+        <v>19</v>
+      </c>
+      <c r="C78" t="s">
         <v>24</v>
       </c>
-      <c r="B78" t="s">
-        <v>7</v>
-      </c>
-      <c r="C78" t="s">
-        <v>6</v>
-      </c>
       <c r="D78" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E78" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="F78" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>20</v>
+      </c>
+      <c r="B79" t="s">
+        <v>19</v>
+      </c>
+      <c r="C79" t="s">
+        <v>4</v>
+      </c>
+      <c r="D79" t="s">
+        <v>21</v>
+      </c>
+      <c r="E79" t="s">
+        <v>29</v>
+      </c>
+      <c r="F79" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>16</v>
+      </c>
+      <c r="B80" t="s">
+        <v>19</v>
+      </c>
+      <c r="C80" t="s">
+        <v>33</v>
+      </c>
+      <c r="D80" t="s">
+        <v>28</v>
+      </c>
+      <c r="E80" t="s">
+        <v>30</v>
+      </c>
+      <c r="F80" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>16</v>
+      </c>
+      <c r="B81" t="s">
+        <v>17</v>
+      </c>
+      <c r="C81" t="s">
+        <v>33</v>
+      </c>
+      <c r="D81" t="s">
+        <v>28</v>
+      </c>
+      <c r="E81" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>16</v>
+      </c>
+      <c r="B82" t="s">
+        <v>19</v>
+      </c>
+      <c r="C82" t="s">
+        <v>33</v>
+      </c>
+      <c r="D82" t="s">
+        <v>28</v>
+      </c>
+      <c r="E82" t="s">
+        <v>1</v>
+      </c>
+      <c r="F82" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>16</v>
+      </c>
+      <c r="B83" t="s">
+        <v>17</v>
+      </c>
+      <c r="C83" t="s">
+        <v>33</v>
+      </c>
+      <c r="D83" t="s">
+        <v>18</v>
+      </c>
+      <c r="E83" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>16</v>
+      </c>
+      <c r="B84" t="s">
+        <v>19</v>
+      </c>
+      <c r="C84" t="s">
+        <v>33</v>
+      </c>
+      <c r="D84" t="s">
+        <v>18</v>
+      </c>
+      <c r="E84" t="s">
+        <v>2</v>
+      </c>
+      <c r="F84" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>16</v>
+      </c>
+      <c r="B85" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85" t="s">
+        <v>32</v>
+      </c>
+      <c r="E85" t="s">
+        <v>30</v>
+      </c>
+      <c r="F85" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="15" priority="11" operator="containsText" text="CoordAux">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="CoordAux">
       <formula>NOT(ISERROR(SEARCH("CoordAux",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="CoordFsm">
+    <cfRule type="containsText" dxfId="6" priority="13" operator="containsText" text="CoordFsm">
       <formula>NOT(ISERROR(SEARCH("CoordFsm",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="13" priority="6" operator="containsText" text="aux">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="aux">
       <formula>NOT(ISERROR(SEARCH("aux",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="EVT_FSM_SUPERSTATE_EXIT">
+      <formula>NOT(ISERROR(SEARCH("EVT_FSM_SUPERSTATE_EXIT",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="EVT_FSM_SUPERSTATE_ENTRY">
+      <formula>NOT(ISERROR(SEARCH("EVT_FSM_SUPERSTATE_ENTRY",E1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"EVT_FSM_ENTRY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="10" operator="equal">
       <formula>"EVT_FSM_EXIT"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="EVT_FSM_SUPERSTATE_ENTRY">
-      <formula>NOT(ISERROR(SEARCH("EVT_FSM_SUPERSTATE_ENTRY",E1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="EVT_FSM_SUPERSTATE_EXIT">
-      <formula>NOT(ISERROR(SEARCH("EVT_FSM_SUPERSTATE_EXIT",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F1048576">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>$C1="aux"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>